<commit_message>
Edit database in excel
</commit_message>
<xml_diff>
--- a/database/Database-In-More-Detail.xlsx
+++ b/database/Database-In-More-Detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BookStore-MultiPlatform\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AEAEC7-675D-4F6C-960E-51C6372AFC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDB2EC3-DFCD-4C08-8812-A9CFC3F750DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
   </bookViews>
@@ -301,9 +301,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -313,6 +310,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,602 +628,602 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D19A7-44BD-47E8-BCBA-FDF3CC1D1199}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="G1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+    <row r="9" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="10" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G10" s="3">
         <v>2</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="K10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="11" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G11" s="3">
         <v>3</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="K11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="K14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+    <row r="15" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G15" s="3">
         <v>1</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="J15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+    <row r="16" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G16" s="3">
         <v>2</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G17" s="3">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="K17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="K20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+    <row r="21" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G21" s="3">
         <v>1</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="I21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="K21" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G22" s="3">
         <v>2</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="I22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="J22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="K22" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+    <row r="23" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G23" s="3">
         <v>3</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="H23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="I23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="J23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="K23" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+    <row r="24" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G24" s="3">
         <v>4</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="H24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="I24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="J24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="K24" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+    <row r="25" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G25" s="3">
         <v>5</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="H25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="I25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="J25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="K25" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+    <row r="26" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="3">
         <v>6</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="H26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="I26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="J26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="K26" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+    <row r="27" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G27" s="3">
         <v>7</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="H27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="I27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="J27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="K27" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    <row r="28" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G28" s="3">
         <v>8</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="H28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="I28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="J28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="K28" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+    <row r="29" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G29" s="3">
         <v>9</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="I29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="J29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="K29" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+    <row r="30" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G30" s="3">
         <v>10</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="H30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="I30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="J30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="K30" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+    <row r="31" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G31" s="3">
         <v>11</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="H31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="I31" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="J31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="K31" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="I34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="J34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="K34" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+    <row r="35" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G35" s="3">
         <v>1</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="H35" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="I35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="J35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="K35" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+    <row r="36" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G36" s="3">
         <v>2</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="H36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="I36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="J36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G37" s="3">
         <v>3</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="H37" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G38" s="3">
         <v>4</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="H38" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G39" s="3">
         <v>5</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="H39" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G40" s="3">
         <v>6</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="H40" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G41" s="3">
         <v>7</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="H41" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="7:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G42" s="3">
         <v>8</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="H42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="I42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="J42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="K42" s="3" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish design database, diagram and generate script in SQL Server
</commit_message>
<xml_diff>
--- a/database/Database-In-More-Detail.xlsx
+++ b/database/Database-In-More-Detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BookStore-API\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2D36E9-0205-4025-B402-0510CD132174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C355FEAB-B1D9-46C3-9D54-8525C325DFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="126">
   <si>
     <t>Publisher</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>OrderItem</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>FK</t>
   </si>
 </sst>
 </file>
@@ -593,20 +599,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -615,6 +615,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -933,19 +939,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D19A7-44BD-47E8-BCBA-FDF3CC1D1199}">
   <dimension ref="G1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N66" sqref="N66"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="12"/>
-    <col min="7" max="7" width="3.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="89.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="3.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="89.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="7:11" x14ac:dyDescent="0.25">
@@ -1331,7 +1337,7 @@
       <c r="H28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="10" t="s">
         <v>36</v>
       </c>
       <c r="J28" s="2" t="s">
@@ -1365,7 +1371,7 @@
       <c r="H30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="I30" s="10" t="s">
         <v>38</v>
       </c>
       <c r="J30" s="2" t="s">
@@ -1494,7 +1500,7 @@
         <v>53</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>14</v>
@@ -1656,7 +1662,7 @@
         <v>53</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>14</v>
@@ -1690,7 +1696,7 @@
         <v>67</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>21</v>
@@ -1854,7 +1860,7 @@
       <c r="I63" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J63" s="13" t="s">
+      <c r="J63" s="10" t="s">
         <v>14</v>
       </c>
       <c r="K63" s="2" t="s">
@@ -1871,7 +1877,7 @@
       <c r="I64" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J64" s="13" t="s">
+      <c r="J64" s="10" t="s">
         <v>83</v>
       </c>
       <c r="K64" s="2" t="s">
@@ -1885,10 +1891,10 @@
       <c r="H65" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I65" s="13" t="s">
+      <c r="I65" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J65" s="13" t="s">
+      <c r="J65" s="10" t="s">
         <v>84</v>
       </c>
       <c r="K65" s="2" t="s">
@@ -1902,10 +1908,10 @@
       <c r="H66" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I66" s="13" t="s">
+      <c r="I66" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="J66" s="13" t="s">
+      <c r="J66" s="10" t="s">
         <v>85</v>
       </c>
       <c r="K66" s="2" t="s">
@@ -1919,10 +1925,10 @@
       <c r="H67" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I67" s="13" t="s">
+      <c r="I67" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J67" s="13" t="s">
+      <c r="J67" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K67" s="2" t="s">
@@ -1947,13 +1953,13 @@
       </c>
     </row>
     <row r="70" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G70" s="14" t="s">
+      <c r="G70" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="16"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="14"/>
     </row>
     <row r="71" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G71" s="4" t="s">
@@ -2034,7 +2040,7 @@
         <v>18</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>39</v>
+        <v>125</v>
       </c>
       <c r="K75" s="8" t="s">
         <v>106</v>
@@ -2064,7 +2070,7 @@
       <c r="H77" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I77" s="13" t="s">
+      <c r="I77" s="10" t="s">
         <v>102</v>
       </c>
       <c r="J77" s="8" t="s">
@@ -2081,7 +2087,7 @@
       <c r="H78" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I78" s="13" t="s">
+      <c r="I78" s="10" t="s">
         <v>102</v>
       </c>
       <c r="J78" s="8" t="s">
@@ -2098,7 +2104,7 @@
       <c r="H79" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I79" s="13" t="s">
+      <c r="I79" s="10" t="s">
         <v>102</v>
       </c>
       <c r="J79" s="8" t="s">
@@ -2115,7 +2121,7 @@
       <c r="H80" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I80" s="13" t="s">
+      <c r="I80" s="10" t="s">
         <v>20</v>
       </c>
       <c r="J80" s="8" t="s">
@@ -2132,7 +2138,7 @@
       <c r="H81" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I81" s="13" t="s">
+      <c r="I81" s="10" t="s">
         <v>101</v>
       </c>
       <c r="J81" s="8"/>
@@ -2158,13 +2164,13 @@
       </c>
     </row>
     <row r="84" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G84" s="14" t="s">
+      <c r="G84" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="H84" s="15"/>
-      <c r="I84" s="15"/>
-      <c r="J84" s="15"/>
-      <c r="K84" s="16"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="14"/>
     </row>
     <row r="85" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G85" s="4" t="s">
@@ -2193,7 +2199,7 @@
       <c r="I86" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J86" s="9" t="s">
+      <c r="J86" s="15" t="s">
         <v>116</v>
       </c>
       <c r="K86" s="8" t="s">
@@ -2210,7 +2216,7 @@
       <c r="I87" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J87" s="10"/>
+      <c r="J87" s="16"/>
       <c r="K87" s="8" t="s">
         <v>118</v>
       </c>
@@ -2222,10 +2228,10 @@
       <c r="H88" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I88" s="13" t="s">
+      <c r="I88" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J88" s="13" t="s">
+      <c r="J88" s="10" t="s">
         <v>86</v>
       </c>
       <c r="K88" s="8" t="s">
@@ -2239,10 +2245,10 @@
       <c r="H89" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I89" s="13" t="s">
+      <c r="I89" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J89" s="13" t="s">
+      <c r="J89" s="10" t="s">
         <v>41</v>
       </c>
       <c r="K89" s="8" t="s">
@@ -2268,16 +2274,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G19:K19"/>
     <mergeCell ref="G44:K44"/>
     <mergeCell ref="G59:K59"/>
     <mergeCell ref="G70:K70"/>
     <mergeCell ref="G84:K84"/>
     <mergeCell ref="J86:J87"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Naming convention: Change snake_case to camelCase
</commit_message>
<xml_diff>
--- a/database/Database-In-More-Detail.xlsx
+++ b/database/Database-In-More-Detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BookStore-API\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C355FEAB-B1D9-46C3-9D54-8525C325DFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AE1905-245B-4147-ABA2-26BF7118DF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>publisher_id</t>
-  </si>
-  <si>
     <t>smallint</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>category_id</t>
-  </si>
-  <si>
     <t>Mã thể loại</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>NOT NULL</t>
   </si>
   <si>
-    <t>is_delete</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -129,12 +120,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>author_id</t>
-  </si>
-  <si>
-    <t>year_of_publication</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -186,15 +171,6 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>family_name</t>
-  </si>
-  <si>
-    <t>given_name</t>
-  </si>
-  <si>
-    <t>date_of_birth</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
@@ -240,12 +216,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>citizen_identification</t>
-  </si>
-  <si>
-    <t>hash_password</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
@@ -267,27 +237,15 @@
     <t>Quyền, 0 = staff, 1 = admin</t>
   </si>
   <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
     <t>condition</t>
   </si>
   <si>
-    <t>discount_percent</t>
-  </si>
-  <si>
     <t>datetime2</t>
   </si>
   <si>
     <t>decimal(3, 2)</t>
   </si>
   <si>
-    <t>NOT NULL, &gt; start_date</t>
-  </si>
-  <si>
     <t>NOT NULL, &gt; 50000</t>
   </si>
   <si>
@@ -312,27 +270,6 @@
     <t>Số lượng</t>
   </si>
   <si>
-    <t>staff_id</t>
-  </si>
-  <si>
-    <t>customer_id</t>
-  </si>
-  <si>
-    <t>promotion_id</t>
-  </si>
-  <si>
-    <t>created_time</t>
-  </si>
-  <si>
-    <t>total_amount</t>
-  </si>
-  <si>
-    <t>sub_total_amount</t>
-  </si>
-  <si>
-    <t>promotion_amount</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -378,12 +315,6 @@
     <t>Ghi chú hóa đơn (khi gặp lỗi)</t>
   </si>
   <si>
-    <t>order_id</t>
-  </si>
-  <si>
-    <t>book_id</t>
-  </si>
-  <si>
     <t>PK, FK</t>
   </si>
   <si>
@@ -412,6 +343,75 @@
   </si>
   <si>
     <t>FK</t>
+  </si>
+  <si>
+    <t>isDeleted</t>
+  </si>
+  <si>
+    <t>categoryId</t>
+  </si>
+  <si>
+    <t>authorId</t>
+  </si>
+  <si>
+    <t>publisherId</t>
+  </si>
+  <si>
+    <t>yearOfPublication</t>
+  </si>
+  <si>
+    <t>familyName</t>
+  </si>
+  <si>
+    <t>givenName</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>citizenIdentification</t>
+  </si>
+  <si>
+    <t>hashPassword</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>NOT NULL, &gt; startDate</t>
+  </si>
+  <si>
+    <t>discountPercent</t>
+  </si>
+  <si>
+    <t>staffId</t>
+  </si>
+  <si>
+    <t>customerId</t>
+  </si>
+  <si>
+    <t>promotionId</t>
+  </si>
+  <si>
+    <t>createdTime</t>
+  </si>
+  <si>
+    <t>totalAmount</t>
+  </si>
+  <si>
+    <t>subTotalAmount</t>
+  </si>
+  <si>
+    <t>promotionAmount</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>bookId</t>
   </si>
 </sst>
 </file>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D19A7-44BD-47E8-BCBA-FDF3CC1D1199}">
   <dimension ref="G1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +956,7 @@
   <sheetData>
     <row r="1" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G1" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
@@ -985,16 +985,16 @@
         <v>1</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="7:11" x14ac:dyDescent="0.25">
@@ -1002,16 +1002,16 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="7:11" x14ac:dyDescent="0.25">
@@ -1019,21 +1019,21 @@
         <v>3</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G7" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -1062,16 +1062,16 @@
         <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="7:11" x14ac:dyDescent="0.25">
@@ -1079,16 +1079,16 @@
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="7:11" x14ac:dyDescent="0.25">
@@ -1096,16 +1096,16 @@
         <v>3</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="7:11" x14ac:dyDescent="0.25">
@@ -1139,16 +1139,16 @@
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="7:11" x14ac:dyDescent="0.25">
@@ -1156,16 +1156,16 @@
         <v>2</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.25">
@@ -1173,21 +1173,21 @@
         <v>3</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G19" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -1216,16 +1216,16 @@
         <v>1</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="7:11" x14ac:dyDescent="0.25">
@@ -1233,16 +1233,16 @@
         <v>2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.25">
@@ -1250,16 +1250,16 @@
         <v>3</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="7:11" x14ac:dyDescent="0.25">
@@ -1267,16 +1267,16 @@
         <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="7:11" x14ac:dyDescent="0.25">
@@ -1284,16 +1284,16 @@
         <v>5</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="7:11" x14ac:dyDescent="0.25">
@@ -1301,16 +1301,16 @@
         <v>6</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="7:11" x14ac:dyDescent="0.25">
@@ -1318,16 +1318,16 @@
         <v>7</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="7:11" x14ac:dyDescent="0.25">
@@ -1335,16 +1335,16 @@
         <v>8</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="K28" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="7:11" x14ac:dyDescent="0.25">
@@ -1352,16 +1352,16 @@
         <v>9</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="7:11" x14ac:dyDescent="0.25">
@@ -1369,16 +1369,16 @@
         <v>10</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="J30" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="7:11" x14ac:dyDescent="0.25">
@@ -1386,21 +1386,21 @@
         <v>11</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G33" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -1429,16 +1429,16 @@
         <v>1</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
@@ -1446,16 +1446,16 @@
         <v>2</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="7:11" x14ac:dyDescent="0.25">
@@ -1463,16 +1463,16 @@
         <v>3</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="7:11" x14ac:dyDescent="0.25">
@@ -1480,16 +1480,16 @@
         <v>4</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="7:11" x14ac:dyDescent="0.25">
@@ -1497,16 +1497,16 @@
         <v>5</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="7:11" x14ac:dyDescent="0.25">
@@ -1514,16 +1514,16 @@
         <v>6</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="7:11" x14ac:dyDescent="0.25">
@@ -1531,16 +1531,16 @@
         <v>7</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="7:11" x14ac:dyDescent="0.25">
@@ -1548,21 +1548,21 @@
         <v>8</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G44" s="11" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
@@ -1591,16 +1591,16 @@
         <v>1</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="7:11" x14ac:dyDescent="0.25">
@@ -1608,16 +1608,16 @@
         <v>2</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="7:11" x14ac:dyDescent="0.25">
@@ -1625,16 +1625,16 @@
         <v>3</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="7:11" x14ac:dyDescent="0.25">
@@ -1642,16 +1642,16 @@
         <v>4</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="7:11" x14ac:dyDescent="0.25">
@@ -1659,16 +1659,16 @@
         <v>5</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="7:11" x14ac:dyDescent="0.25">
@@ -1676,16 +1676,16 @@
         <v>6</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="7:11" x14ac:dyDescent="0.25">
@@ -1693,16 +1693,16 @@
         <v>7</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="7:11" x14ac:dyDescent="0.25">
@@ -1710,16 +1710,16 @@
         <v>8</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="7:11" x14ac:dyDescent="0.25">
@@ -1727,16 +1727,16 @@
         <v>9</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="7:11" x14ac:dyDescent="0.25">
@@ -1744,16 +1744,16 @@
         <v>10</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="7:11" x14ac:dyDescent="0.25">
@@ -1761,16 +1761,16 @@
         <v>11</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="7:11" x14ac:dyDescent="0.25">
@@ -1778,21 +1778,21 @@
         <v>12</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G59" s="11" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
@@ -1821,16 +1821,16 @@
         <v>1</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="7:11" x14ac:dyDescent="0.25">
@@ -1838,16 +1838,16 @@
         <v>2</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="7:11" x14ac:dyDescent="0.25">
@@ -1855,16 +1855,16 @@
         <v>3</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="7:11" x14ac:dyDescent="0.25">
@@ -1872,16 +1872,16 @@
         <v>4</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="7:11" x14ac:dyDescent="0.25">
@@ -1889,16 +1889,16 @@
         <v>5</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="7:11" x14ac:dyDescent="0.25">
@@ -1906,16 +1906,16 @@
         <v>6</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="7:11" x14ac:dyDescent="0.25">
@@ -1923,16 +1923,16 @@
         <v>7</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="7:11" x14ac:dyDescent="0.25">
@@ -1940,21 +1940,21 @@
         <v>8</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G70" s="12" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
@@ -1983,16 +1983,16 @@
         <v>1</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J72" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="7:11" x14ac:dyDescent="0.25">
@@ -2000,16 +2000,16 @@
         <v>2</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="7:11" x14ac:dyDescent="0.25">
@@ -2017,16 +2017,16 @@
         <v>3</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="7:11" x14ac:dyDescent="0.25">
@@ -2034,16 +2034,16 @@
         <v>4</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="K75" s="8" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="7:11" x14ac:dyDescent="0.25">
@@ -2051,16 +2051,16 @@
         <v>5</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="K76" s="8" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="7:11" x14ac:dyDescent="0.25">
@@ -2068,16 +2068,16 @@
         <v>6</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="I77" s="10" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="J77" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="7:11" x14ac:dyDescent="0.25">
@@ -2085,16 +2085,16 @@
         <v>7</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="I78" s="10" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="J78" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="7:11" x14ac:dyDescent="0.25">
@@ -2102,16 +2102,16 @@
         <v>8</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="I79" s="10" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="J79" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K79" s="8" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="7:11" x14ac:dyDescent="0.25">
@@ -2119,16 +2119,16 @@
         <v>9</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="I80" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J80" s="8" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="7:11" x14ac:dyDescent="0.25">
@@ -2136,14 +2136,14 @@
         <v>10</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="I81" s="10" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="8" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="7:11" x14ac:dyDescent="0.25">
@@ -2151,21 +2151,21 @@
         <v>11</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J82" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K82" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="84" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G84" s="12" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
@@ -2194,16 +2194,16 @@
         <v>1</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J86" s="15" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="K86" s="8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="7:11" x14ac:dyDescent="0.25">
@@ -2211,14 +2211,14 @@
         <v>2</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J87" s="16"/>
       <c r="K87" s="8" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="7:11" x14ac:dyDescent="0.25">
@@ -2226,16 +2226,16 @@
         <v>3</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I88" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J88" s="10" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="K88" s="8" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="7:11" x14ac:dyDescent="0.25">
@@ -2243,16 +2243,16 @@
         <v>4</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I89" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J89" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J89" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="K89" s="8" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="7:11" x14ac:dyDescent="0.25">
@@ -2260,30 +2260,30 @@
         <v>5</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J90" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K90" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G44:K44"/>
+    <mergeCell ref="G59:K59"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="G84:K84"/>
+    <mergeCell ref="J86:J87"/>
     <mergeCell ref="G33:K33"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G44:K44"/>
-    <mergeCell ref="G59:K59"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="G84:K84"/>
-    <mergeCell ref="J86:J87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Edit some fields in database and regenerate script
</commit_message>
<xml_diff>
--- a/database/Database-In-More-Detail.xlsx
+++ b/database/Database-In-More-Detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BookStore-API\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AE1905-245B-4147-ABA2-26BF7118DF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2481D9-7E63-407E-B3A9-C9CC6D77D5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="124">
   <si>
     <t>Publisher</t>
   </si>
@@ -222,9 +222,6 @@
     <t>char(12)</t>
   </si>
   <si>
-    <t>NOT NULL, &gt; 18t</t>
-  </si>
-  <si>
     <t>Địa chỉ mail</t>
   </si>
   <si>
@@ -244,9 +241,6 @@
   </si>
   <si>
     <t>decimal(3, 2)</t>
-  </si>
-  <si>
-    <t>NOT NULL, &gt; 50000</t>
   </si>
   <si>
     <t>NOT NULL, &gt; 0.0</t>
@@ -939,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D19A7-44BD-47E8-BCBA-FDF3CC1D1199}">
   <dimension ref="G1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" topLeftCell="D66" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I85" sqref="I85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1013,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>17</v>
@@ -1096,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>17</v>
@@ -1173,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>17</v>
@@ -1267,7 +1261,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>15</v>
@@ -1284,7 +1278,7 @@
         <v>5</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>15</v>
@@ -1301,7 +1295,7 @@
         <v>6</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>15</v>
@@ -1318,7 +1312,7 @@
         <v>7</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>6</v>
@@ -1327,7 +1321,7 @@
         <v>35</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="7:11" x14ac:dyDescent="0.25">
@@ -1386,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>17</v>
@@ -1446,7 +1440,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>48</v>
@@ -1463,7 +1457,7 @@
         <v>3</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>49</v>
@@ -1480,7 +1474,7 @@
         <v>4</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>51</v>
@@ -1548,7 +1542,7 @@
         <v>8</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>17</v>
@@ -1608,7 +1602,7 @@
         <v>2</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>48</v>
@@ -1625,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>49</v>
@@ -1642,13 +1636,13 @@
         <v>4</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>51</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>55</v>
@@ -1696,13 +1690,13 @@
         <v>59</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="7:11" x14ac:dyDescent="0.25">
@@ -1710,7 +1704,7 @@
         <v>8</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>61</v>
@@ -1719,7 +1713,7 @@
         <v>18</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="7:11" x14ac:dyDescent="0.25">
@@ -1727,7 +1721,7 @@
         <v>9</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>32</v>
@@ -1736,7 +1730,7 @@
         <v>12</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="7:11" x14ac:dyDescent="0.25">
@@ -1753,7 +1747,7 @@
         <v>19</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="7:11" x14ac:dyDescent="0.25">
@@ -1778,7 +1772,7 @@
         <v>12</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>17</v>
@@ -1792,7 +1786,7 @@
     </row>
     <row r="59" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G59" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
@@ -1855,16 +1849,16 @@
         <v>3</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J63" s="10" t="s">
         <v>12</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="7:11" x14ac:dyDescent="0.25">
@@ -1872,16 +1866,16 @@
         <v>4</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="7:11" x14ac:dyDescent="0.25">
@@ -1889,16 +1883,16 @@
         <v>5</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I65" s="10" t="s">
         <v>31</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="7:11" x14ac:dyDescent="0.25">
@@ -1906,16 +1900,16 @@
         <v>6</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I66" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J66" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="J66" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="K66" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="7:11" x14ac:dyDescent="0.25">
@@ -1932,7 +1926,7 @@
         <v>37</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="7:11" x14ac:dyDescent="0.25">
@@ -1940,7 +1934,7 @@
         <v>8</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>17</v>
@@ -1954,7 +1948,7 @@
     </row>
     <row r="70" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G70" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
@@ -2000,7 +1994,7 @@
         <v>2</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I73" s="8" t="s">
         <v>15</v>
@@ -2009,7 +2003,7 @@
         <v>34</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="7:11" x14ac:dyDescent="0.25">
@@ -2017,7 +2011,7 @@
         <v>3</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I74" s="8" t="s">
         <v>15</v>
@@ -2026,7 +2020,7 @@
         <v>34</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="7:11" x14ac:dyDescent="0.25">
@@ -2034,16 +2028,16 @@
         <v>4</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K75" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="7:11" x14ac:dyDescent="0.25">
@@ -2051,16 +2045,16 @@
         <v>5</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K76" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="7:11" x14ac:dyDescent="0.25">
@@ -2068,16 +2062,16 @@
         <v>6</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I77" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J77" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="7:11" x14ac:dyDescent="0.25">
@@ -2085,16 +2079,16 @@
         <v>7</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I78" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J78" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="7:11" x14ac:dyDescent="0.25">
@@ -2102,16 +2096,16 @@
         <v>8</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I79" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J79" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K79" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="7:11" x14ac:dyDescent="0.25">
@@ -2119,16 +2113,16 @@
         <v>9</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I80" s="10" t="s">
         <v>17</v>
       </c>
       <c r="J80" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="7:11" x14ac:dyDescent="0.25">
@@ -2136,14 +2130,14 @@
         <v>10</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I81" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="7:11" x14ac:dyDescent="0.25">
@@ -2151,7 +2145,7 @@
         <v>11</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I82" s="8" t="s">
         <v>17</v>
@@ -2165,7 +2159,7 @@
     </row>
     <row r="84" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G84" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
@@ -2194,16 +2188,16 @@
         <v>1</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I86" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J86" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K86" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="7:11" x14ac:dyDescent="0.25">
@@ -2211,14 +2205,14 @@
         <v>2</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J87" s="16"/>
       <c r="K87" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="7:11" x14ac:dyDescent="0.25">
@@ -2232,10 +2226,10 @@
         <v>6</v>
       </c>
       <c r="J88" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K88" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="7:11" x14ac:dyDescent="0.25">
@@ -2252,7 +2246,7 @@
         <v>36</v>
       </c>
       <c r="K89" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90" spans="7:11" x14ac:dyDescent="0.25">
@@ -2260,7 +2254,7 @@
         <v>5</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I90" s="8" t="s">
         <v>17</v>
@@ -2274,16 +2268,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G19:K19"/>
     <mergeCell ref="G44:K44"/>
     <mergeCell ref="G59:K59"/>
     <mergeCell ref="G70:K70"/>
     <mergeCell ref="G84:K84"/>
     <mergeCell ref="J86:J87"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Insert isActived field into Staff to check staff activation
</commit_message>
<xml_diff>
--- a/database/Database-In-More-Detail.xlsx
+++ b/database/Database-In-More-Detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BookStore-API\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2481D9-7E63-407E-B3A9-C9CC6D77D5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350254F6-5C9C-4AC7-9E82-16C2CEDB3BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="126">
   <si>
     <t>Publisher</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>bookId</t>
+  </si>
+  <si>
+    <t>isActived</t>
+  </si>
+  <si>
+    <t>Trạng thái kích hoạt tài khoản, 0 = chưa, 1 = rồi</t>
   </si>
 </sst>
 </file>
@@ -931,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D19A7-44BD-47E8-BCBA-FDF3CC1D1199}">
-  <dimension ref="G1:K90"/>
+  <dimension ref="G1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D66" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I85" sqref="I85"/>
+    <sheetView tabSelected="1" topLeftCell="D39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,7 +1778,7 @@
         <v>12</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>17</v>
@@ -1781,237 +1787,237 @@
         <v>19</v>
       </c>
       <c r="K57" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G58" s="2">
+        <v>13</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K58" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G59" s="11" t="s">
+    <row r="60" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G60" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-    </row>
-    <row r="60" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G60" s="1" t="s">
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+    </row>
+    <row r="61" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G61" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H60" s="1" t="s">
+      <c r="H61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="I61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="J61" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="K61" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G61" s="2">
-        <v>1</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="62" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G62" s="2">
-        <v>2</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G63" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J63" s="10" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G64" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>67</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G65" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I65" s="10" t="s">
-        <v>31</v>
+        <v>112</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G66" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G67" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G68" s="2">
+        <v>7</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J68" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G69" s="2">
         <v>8</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K68" s="2" t="s">
+      <c r="K69" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G70" s="12" t="s">
+    <row r="71" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G71" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="14"/>
-    </row>
-    <row r="71" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G71" s="4" t="s">
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="14"/>
+    </row>
+    <row r="72" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G72" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H72" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I72" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J71" s="5" t="s">
+      <c r="J72" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K71" s="5" t="s">
+      <c r="K72" s="5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G72" s="6">
-        <v>1</v>
-      </c>
-      <c r="H72" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I72" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J72" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K72" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="73" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G73" s="6">
-        <v>2</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>115</v>
+        <v>1</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="I73" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J73" s="2" t="s">
-        <v>34</v>
+      <c r="J73" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G74" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I74" s="8" t="s">
         <v>15</v>
@@ -2020,66 +2026,66 @@
         <v>34</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G75" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="K75" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G76" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J76" s="8" t="s">
-        <v>80</v>
+        <v>15</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="K76" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G77" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I77" s="10" t="s">
-        <v>79</v>
+        <v>118</v>
+      </c>
+      <c r="I77" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="J77" s="8" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G78" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I78" s="10" t="s">
         <v>79</v>
@@ -2088,15 +2094,15 @@
         <v>12</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G79" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I79" s="10" t="s">
         <v>79</v>
@@ -2105,179 +2111,196 @@
         <v>12</v>
       </c>
       <c r="K79" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G80" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="I80" s="10" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="J80" s="8" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G81" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I81" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J81" s="8"/>
+        <v>17</v>
+      </c>
+      <c r="J81" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="K81" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G82" s="6">
+        <v>10</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J82" s="8"/>
+      <c r="K82" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G83" s="6">
         <v>11</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H83" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I82" s="8" t="s">
+      <c r="I83" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J82" s="8" t="s">
+      <c r="J83" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="8" t="s">
+      <c r="K83" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G84" s="12" t="s">
+    <row r="85" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G85" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="14"/>
-    </row>
-    <row r="85" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G85" s="4" t="s">
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="14"/>
+    </row>
+    <row r="86" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G86" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H85" s="5" t="s">
+      <c r="H86" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I85" s="5" t="s">
+      <c r="I86" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J85" s="5" t="s">
+      <c r="J86" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K85" s="5" t="s">
+      <c r="K86" s="5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G86" s="6">
-        <v>1</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I86" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J86" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="K86" s="8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="87" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G87" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J87" s="16"/>
+      <c r="J87" s="15" t="s">
+        <v>91</v>
+      </c>
       <c r="K87" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G88" s="6">
-        <v>3</v>
-      </c>
-      <c r="H88" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I88" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J88" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I88" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J88" s="16"/>
       <c r="K88" s="8" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="89" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G89" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I89" s="10" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="J89" s="10" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="K89" s="8" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G90" s="6">
+        <v>4</v>
+      </c>
+      <c r="H90" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J90" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K90" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G91" s="6">
         <v>5</v>
       </c>
-      <c r="H90" s="8" t="s">
+      <c r="H91" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="I90" s="8" t="s">
+      <c r="I91" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J90" s="8" t="s">
+      <c r="J91" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K90" s="8" t="s">
+      <c r="K91" s="8" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G44:K44"/>
+    <mergeCell ref="G60:K60"/>
+    <mergeCell ref="G71:K71"/>
+    <mergeCell ref="G85:K85"/>
+    <mergeCell ref="J87:J88"/>
     <mergeCell ref="G33:K33"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G44:K44"/>
-    <mergeCell ref="G59:K59"/>
-    <mergeCell ref="G70:K70"/>
-    <mergeCell ref="G84:K84"/>
-    <mergeCell ref="J86:J87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>